<commit_message>
Conducted more interview testing
</commit_message>
<xml_diff>
--- a/visualisation/excel/Consistency-Test.xlsx
+++ b/visualisation/excel/Consistency-Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kent\University Of Kent UK\Projects\Disso\Screening-LLM\visualisation\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f47c0893c577065/Cross Device/Work/Project/Code/Screening-LLM/visualisation/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BDCB40-B502-4869-9EFA-B9A9AEA376E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{B8BDCB40-B502-4869-9EFA-B9A9AEA376E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0250B560-9E85-4843-9C52-3DB001E7DD14}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="0" windowWidth="19200" windowHeight="9970" xr2:uid="{2CBF5892-813D-4C9A-857D-999A29FFE851}"/>
+    <workbookView xWindow="4890" yWindow="2190" windowWidth="21600" windowHeight="11385" xr2:uid="{2CBF5892-813D-4C9A-857D-999A29FFE851}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Interview</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>1724629705-RAG-Good</t>
+  </si>
+  <si>
+    <t>Niranjan</t>
+  </si>
+  <si>
+    <t>1725184560-ITSE-Bad</t>
   </si>
 </sst>
 </file>
@@ -443,22 +449,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D3878F-45EE-418E-B997-8A510AA020C7}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -475,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -492,7 +498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -509,7 +515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -526,7 +532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -543,7 +549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -560,7 +566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -575,6 +581,39 @@
       </c>
       <c r="E7">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning repo to push
</commit_message>
<xml_diff>
--- a/visualisation/excel/Consistency-Test.xlsx
+++ b/visualisation/excel/Consistency-Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kent\University Of Kent UK\Projects\Disso\Screening-LLM\visualisation\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BDCB40-B502-4869-9EFA-B9A9AEA376E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98269D8E-BC6C-4ED3-8648-11BBCAA37E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="0" windowWidth="19200" windowHeight="9970" xr2:uid="{2CBF5892-813D-4C9A-857D-999A29FFE851}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{2CBF5892-813D-4C9A-857D-999A29FFE851}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,22 +56,22 @@
     <t>Debapratim</t>
   </si>
   <si>
-    <t>1724531512-Receptionist-Mid</t>
-  </si>
-  <si>
     <t>1724530742-Receptionist-Good</t>
   </si>
   <si>
     <t>1724532643-Receptionist-Bad</t>
   </si>
   <si>
-    <t>1724632240-RAG-Mid</t>
-  </si>
-  <si>
     <t>1724715512-RAG-Bad</t>
   </si>
   <si>
     <t>1724629705-RAG-Good</t>
+  </si>
+  <si>
+    <t>1725397919-RAG-Average</t>
+  </si>
+  <si>
+    <t>1725380262-Receptionist-Average</t>
   </si>
 </sst>
 </file>
@@ -446,13 +446,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
@@ -480,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -497,13 +497,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -514,7 +514,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -531,7 +531,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -548,13 +548,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -565,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>9</v>

</xml_diff>